<commit_message>
Upload your own update
</commit_message>
<xml_diff>
--- a/Backend/results/17229644778933183683/aggregated_df.xlsx
+++ b/Backend/results/17229644778933183683/aggregated_df.xlsx
@@ -462,13 +462,13 @@
         </is>
       </c>
       <c r="B2" t="n">
-        <v>40</v>
+        <v>1546</v>
       </c>
       <c r="C2" t="n">
-        <v>14.17708333333333</v>
+        <v>248.0625</v>
       </c>
       <c r="D2" t="n">
-        <v>25.82291666666667</v>
+        <v>1297.9375</v>
       </c>
     </row>
     <row r="3">
@@ -478,13 +478,13 @@
         </is>
       </c>
       <c r="B3" t="n">
-        <v>43</v>
+        <v>1574</v>
       </c>
       <c r="C3" t="n">
-        <v>12.9375</v>
+        <v>262.3541666666667</v>
       </c>
       <c r="D3" t="n">
-        <v>30.0625</v>
+        <v>1311.645833333333</v>
       </c>
     </row>
     <row r="4">
@@ -494,13 +494,13 @@
         </is>
       </c>
       <c r="B4" t="n">
-        <v>41</v>
+        <v>1552</v>
       </c>
       <c r="C4" t="n">
-        <v>11.86458333333333</v>
+        <v>252.1458333333333</v>
       </c>
       <c r="D4" t="n">
-        <v>29.13541666666667</v>
+        <v>1299.854166666667</v>
       </c>
     </row>
     <row r="5">
@@ -510,13 +510,13 @@
         </is>
       </c>
       <c r="B5" t="n">
-        <v>49</v>
+        <v>1664</v>
       </c>
       <c r="C5" t="n">
-        <v>16.28125</v>
+        <v>359.75</v>
       </c>
       <c r="D5" t="n">
-        <v>32.71875</v>
+        <v>1304.25</v>
       </c>
     </row>
     <row r="6">
@@ -526,13 +526,13 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>59</v>
+        <v>1496</v>
       </c>
       <c r="C6" t="n">
-        <v>27.46875</v>
+        <v>295.1041666666667</v>
       </c>
       <c r="D6" t="n">
-        <v>31.53125</v>
+        <v>1200.895833333333</v>
       </c>
     </row>
     <row r="7">
@@ -542,13 +542,13 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>60</v>
+        <v>1520</v>
       </c>
       <c r="C7" t="n">
-        <v>23.61458333333334</v>
+        <v>354.6875</v>
       </c>
       <c r="D7" t="n">
-        <v>36.38541666666666</v>
+        <v>1165.3125</v>
       </c>
     </row>
     <row r="8">
@@ -558,13 +558,13 @@
         </is>
       </c>
       <c r="B8" t="n">
-        <v>69</v>
+        <v>1384</v>
       </c>
       <c r="C8" t="n">
-        <v>26.17708333333334</v>
+        <v>243.2291666666667</v>
       </c>
       <c r="D8" t="n">
-        <v>42.82291666666666</v>
+        <v>1140.770833333333</v>
       </c>
     </row>
     <row r="9">
@@ -574,13 +574,13 @@
         </is>
       </c>
       <c r="B9" t="n">
-        <v>67</v>
+        <v>1382</v>
       </c>
       <c r="C9" t="n">
-        <v>23.75</v>
+        <v>255.4375</v>
       </c>
       <c r="D9" t="n">
-        <v>43.25</v>
+        <v>1126.5625</v>
       </c>
     </row>
     <row r="10">
@@ -590,13 +590,13 @@
         </is>
       </c>
       <c r="B10" t="n">
-        <v>64</v>
+        <v>1406</v>
       </c>
       <c r="C10" t="n">
-        <v>16.57291666666666</v>
+        <v>251.2291666666667</v>
       </c>
       <c r="D10" t="n">
-        <v>47.42708333333334</v>
+        <v>1154.770833333333</v>
       </c>
     </row>
     <row r="11">
@@ -606,13 +606,13 @@
         </is>
       </c>
       <c r="B11" t="n">
-        <v>62</v>
+        <v>1420</v>
       </c>
       <c r="C11" t="n">
-        <v>22.71875</v>
+        <v>270.1041666666667</v>
       </c>
       <c r="D11" t="n">
-        <v>39.28125</v>
+        <v>1149.895833333333</v>
       </c>
     </row>
     <row r="12">
@@ -622,13 +622,13 @@
         </is>
       </c>
       <c r="B12" t="n">
-        <v>49</v>
+        <v>1530</v>
       </c>
       <c r="C12" t="n">
-        <v>14.9375</v>
+        <v>255.4375</v>
       </c>
       <c r="D12" t="n">
-        <v>34.0625</v>
+        <v>1274.5625</v>
       </c>
     </row>
     <row r="13">
@@ -638,13 +638,13 @@
         </is>
       </c>
       <c r="B13" t="n">
-        <v>48</v>
+        <v>1480</v>
       </c>
       <c r="C13" t="n">
-        <v>15.46875</v>
+        <v>242.8333333333333</v>
       </c>
       <c r="D13" t="n">
-        <v>32.53125</v>
+        <v>1237.166666666667</v>
       </c>
     </row>
   </sheetData>

</xml_diff>